<commit_message>
master series rates update
</commit_message>
<xml_diff>
--- a/Inputs/Pacific_Cross_Master_Series/rateSheet.xlsx
+++ b/Inputs/Pacific_Cross_Master_Series/rateSheet.xlsx
@@ -321,11 +321,11 @@
   </sheetPr>
   <dimension ref="A1:Q1031"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A296" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H299" activeCellId="0" sqref="H299"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A298" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G301" activeCellId="0" sqref="G301"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.47"/>
@@ -2111,7 +2111,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="7" t="s">
         <v>12</v>
       </c>
@@ -2129,7 +2129,7 @@
         <v>5</v>
       </c>
       <c r="G50" s="10" t="n">
-        <v>26552800</v>
+        <v>33191000</v>
       </c>
       <c r="H50" s="5" t="s">
         <v>22</v>
@@ -2147,7 +2147,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="7" t="s">
         <v>12</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>18</v>
       </c>
       <c r="G51" s="10" t="n">
-        <v>23822400</v>
+        <v>29778000</v>
       </c>
       <c r="H51" s="5" t="s">
         <v>22</v>
@@ -2183,7 +2183,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="7" t="s">
         <v>12</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>25</v>
       </c>
       <c r="G52" s="10" t="n">
-        <v>33795200</v>
+        <v>42244000</v>
       </c>
       <c r="H52" s="5" t="s">
         <v>22</v>
@@ -2219,7 +2219,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="7" t="s">
         <v>12</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>30</v>
       </c>
       <c r="G53" s="10" t="n">
-        <v>36352800</v>
+        <v>45441000</v>
       </c>
       <c r="H53" s="5" t="s">
         <v>22</v>
@@ -2255,7 +2255,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="7" t="s">
         <v>12</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>35</v>
       </c>
       <c r="G54" s="10" t="n">
-        <v>38967200</v>
+        <v>48709000</v>
       </c>
       <c r="H54" s="5" t="s">
         <v>22</v>
@@ -2291,7 +2291,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="7" t="s">
         <v>12</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>40</v>
       </c>
       <c r="G55" s="10" t="n">
-        <v>41652800</v>
+        <v>52066000</v>
       </c>
       <c r="H55" s="5" t="s">
         <v>22</v>
@@ -2327,7 +2327,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="7" t="s">
         <v>12</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>45</v>
       </c>
       <c r="G56" s="10" t="n">
-        <v>44388000</v>
+        <v>55485000</v>
       </c>
       <c r="H56" s="5" t="s">
         <v>22</v>
@@ -2363,7 +2363,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="7" t="s">
         <v>12</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>50</v>
       </c>
       <c r="G57" s="10" t="n">
-        <v>49760000</v>
+        <v>62200000</v>
       </c>
       <c r="H57" s="5" t="s">
         <v>22</v>
@@ -2399,7 +2399,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="7" t="s">
         <v>12</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>55</v>
       </c>
       <c r="G58" s="10" t="n">
-        <v>55236000</v>
+        <v>69045000</v>
       </c>
       <c r="H58" s="5" t="s">
         <v>22</v>
@@ -2435,7 +2435,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="7" t="s">
         <v>12</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>60</v>
       </c>
       <c r="G59" s="10" t="n">
-        <v>68027200</v>
+        <v>85034000</v>
       </c>
       <c r="H59" s="5" t="s">
         <v>22</v>
@@ -2471,7 +2471,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="7" t="s">
         <v>12</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>65</v>
       </c>
       <c r="G60" s="11" t="n">
-        <v>81638400</v>
+        <v>102048000</v>
       </c>
       <c r="H60" s="5" t="s">
         <v>22</v>
@@ -2507,7 +2507,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="7" t="s">
         <v>12</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>70</v>
       </c>
       <c r="G61" s="11" t="n">
-        <v>122484800</v>
+        <v>153106000</v>
       </c>
       <c r="H61" s="5" t="s">
         <v>22</v>
@@ -2543,7 +2543,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="7" t="s">
         <v>12</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>75</v>
       </c>
       <c r="G62" s="11" t="n">
-        <v>169043200</v>
+        <v>211304000</v>
       </c>
       <c r="H62" s="5" t="s">
         <v>22</v>
@@ -2579,7 +2579,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="7" t="s">
         <v>12</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>80</v>
       </c>
       <c r="G63" s="11" t="n">
-        <v>233248800</v>
+        <v>291561000</v>
       </c>
       <c r="H63" s="5" t="s">
         <v>22</v>
@@ -2615,7 +2615,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="7" t="s">
         <v>12</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>85</v>
       </c>
       <c r="G64" s="11" t="n">
-        <v>321860800</v>
+        <v>402326000</v>
       </c>
       <c r="H64" s="5" t="s">
         <v>22</v>
@@ -2651,7 +2651,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="7" t="s">
         <v>12</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>90</v>
       </c>
       <c r="G65" s="11" t="n">
-        <v>444148800</v>
+        <v>555186000</v>
       </c>
       <c r="H65" s="5" t="s">
         <v>22</v>
@@ -2687,7 +2687,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="7" t="s">
         <v>20</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>5</v>
       </c>
       <c r="G66" s="10" t="n">
-        <v>28425600</v>
+        <v>35532000</v>
       </c>
       <c r="H66" s="5" t="s">
         <v>22</v>
@@ -2723,7 +2723,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="7" t="s">
         <v>20</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>18</v>
       </c>
       <c r="G67" s="10" t="n">
-        <v>24713600</v>
+        <v>30892000</v>
       </c>
       <c r="H67" s="5" t="s">
         <v>22</v>
@@ -2759,7 +2759,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="7" t="s">
         <v>20</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>25</v>
       </c>
       <c r="G68" s="10" t="n">
-        <v>40246400</v>
+        <v>50308000</v>
       </c>
       <c r="H68" s="5" t="s">
         <v>22</v>
@@ -2795,7 +2795,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="7" t="s">
         <v>20</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>30</v>
       </c>
       <c r="G69" s="10" t="n">
-        <v>43264000</v>
+        <v>54080000</v>
       </c>
       <c r="H69" s="5" t="s">
         <v>22</v>
@@ -2831,7 +2831,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="7" t="s">
         <v>20</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>35</v>
       </c>
       <c r="G70" s="10" t="n">
-        <v>46282400</v>
+        <v>57853000</v>
       </c>
       <c r="H70" s="5" t="s">
         <v>22</v>
@@ -2867,7 +2867,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="7" t="s">
         <v>20</v>
       </c>
@@ -2885,7 +2885,7 @@
         <v>40</v>
       </c>
       <c r="G71" s="10" t="n">
-        <v>49477600</v>
+        <v>61847000</v>
       </c>
       <c r="H71" s="5" t="s">
         <v>22</v>
@@ -2903,7 +2903,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="7" t="s">
         <v>20</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>45</v>
       </c>
       <c r="G72" s="10" t="n">
-        <v>51963200</v>
+        <v>64954000</v>
       </c>
       <c r="H72" s="5" t="s">
         <v>22</v>
@@ -2939,7 +2939,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="7" t="s">
         <v>20</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>50</v>
       </c>
       <c r="G73" s="10" t="n">
-        <v>58791200</v>
+        <v>73489000</v>
       </c>
       <c r="H73" s="5" t="s">
         <v>22</v>
@@ -2975,7 +2975,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="7" t="s">
         <v>20</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>55</v>
       </c>
       <c r="G74" s="10" t="n">
-        <v>65906400</v>
+        <v>82383000</v>
       </c>
       <c r="H74" s="5" t="s">
         <v>22</v>
@@ -3011,7 +3011,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="7" t="s">
         <v>20</v>
       </c>
@@ -3029,7 +3029,7 @@
         <v>60</v>
       </c>
       <c r="G75" s="11" t="n">
-        <v>81123200</v>
+        <v>101404000</v>
       </c>
       <c r="H75" s="5" t="s">
         <v>22</v>
@@ -3047,7 +3047,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="7" t="s">
         <v>20</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>65</v>
       </c>
       <c r="G76" s="11" t="n">
-        <v>97348000</v>
+        <v>121685000</v>
       </c>
       <c r="H76" s="5" t="s">
         <v>22</v>
@@ -3083,7 +3083,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="7" t="s">
         <v>20</v>
       </c>
@@ -3101,7 +3101,7 @@
         <v>70</v>
       </c>
       <c r="G77" s="11" t="n">
-        <v>146005600</v>
+        <v>182507000</v>
       </c>
       <c r="H77" s="5" t="s">
         <v>22</v>
@@ -3119,7 +3119,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="7" t="s">
         <v>20</v>
       </c>
@@ -3137,7 +3137,7 @@
         <v>75</v>
       </c>
       <c r="G78" s="11" t="n">
-        <v>201518400</v>
+        <v>251898000</v>
       </c>
       <c r="H78" s="5" t="s">
         <v>22</v>
@@ -3155,7 +3155,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="7" t="s">
         <v>20</v>
       </c>
@@ -3173,7 +3173,7 @@
         <v>80</v>
       </c>
       <c r="G79" s="11" t="n">
-        <v>278112000</v>
+        <v>347640000</v>
       </c>
       <c r="H79" s="5" t="s">
         <v>22</v>
@@ -3191,7 +3191,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="7" t="s">
         <v>20</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>85</v>
       </c>
       <c r="G80" s="11" t="n">
-        <v>383800000</v>
+        <v>479750000</v>
       </c>
       <c r="H80" s="5" t="s">
         <v>22</v>
@@ -3227,7 +3227,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="7" t="s">
         <v>20</v>
       </c>
@@ -3245,7 +3245,7 @@
         <v>90</v>
       </c>
       <c r="G81" s="11" t="n">
-        <v>529622400</v>
+        <v>662028000</v>
       </c>
       <c r="H81" s="5" t="s">
         <v>22</v>
@@ -3263,7 +3263,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="7" t="s">
         <v>21</v>
       </c>
@@ -3281,7 +3281,7 @@
         <v>5</v>
       </c>
       <c r="G82" s="10" t="n">
-        <v>32547200</v>
+        <v>40684000</v>
       </c>
       <c r="H82" s="5" t="s">
         <v>22</v>
@@ -3299,7 +3299,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="7" t="s">
         <v>21</v>
       </c>
@@ -3317,7 +3317,7 @@
         <v>18</v>
       </c>
       <c r="G83" s="10" t="n">
-        <v>28296000</v>
+        <v>35370000</v>
       </c>
       <c r="H83" s="5" t="s">
         <v>22</v>
@@ -3335,7 +3335,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="7" t="s">
         <v>21</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>25</v>
       </c>
       <c r="G84" s="10" t="n">
-        <v>50938400</v>
+        <v>63673000</v>
       </c>
       <c r="H84" s="5" t="s">
         <v>22</v>
@@ -3371,7 +3371,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="7" t="s">
         <v>21</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>30</v>
       </c>
       <c r="G85" s="10" t="n">
-        <v>54571200</v>
+        <v>68214000</v>
       </c>
       <c r="H85" s="5" t="s">
         <v>22</v>
@@ -3407,7 +3407,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="7" t="s">
         <v>21</v>
       </c>
@@ -3425,7 +3425,7 @@
         <v>35</v>
       </c>
       <c r="G86" s="10" t="n">
-        <v>58254400</v>
+        <v>72818000</v>
       </c>
       <c r="H86" s="5" t="s">
         <v>22</v>
@@ -3443,7 +3443,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="7" t="s">
         <v>21</v>
       </c>
@@ -3461,7 +3461,7 @@
         <v>40</v>
       </c>
       <c r="G87" s="10" t="n">
-        <v>61897600</v>
+        <v>77372000</v>
       </c>
       <c r="H87" s="5" t="s">
         <v>22</v>
@@ -3479,7 +3479,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="7" t="s">
         <v>21</v>
       </c>
@@ -3497,7 +3497,7 @@
         <v>45</v>
       </c>
       <c r="G88" s="10" t="n">
-        <v>66748800</v>
+        <v>83436000</v>
       </c>
       <c r="H88" s="5" t="s">
         <v>22</v>
@@ -3515,7 +3515,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="7" t="s">
         <v>21</v>
       </c>
@@ -3533,7 +3533,7 @@
         <v>50</v>
       </c>
       <c r="G89" s="10" t="n">
-        <v>70485600</v>
+        <v>88107000</v>
       </c>
       <c r="H89" s="5" t="s">
         <v>22</v>
@@ -3551,7 +3551,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="7" t="s">
         <v>21</v>
       </c>
@@ -3569,7 +3569,7 @@
         <v>55</v>
       </c>
       <c r="G90" s="11" t="n">
-        <v>81073600</v>
+        <v>101342000</v>
       </c>
       <c r="H90" s="5" t="s">
         <v>22</v>
@@ -3587,7 +3587,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="7" t="s">
         <v>21</v>
       </c>
@@ -3605,7 +3605,7 @@
         <v>60</v>
       </c>
       <c r="G91" s="11" t="n">
-        <v>91229600</v>
+        <v>114037000</v>
       </c>
       <c r="H91" s="5" t="s">
         <v>22</v>
@@ -3623,7 +3623,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="7" t="s">
         <v>21</v>
       </c>
@@ -3641,7 +3641,7 @@
         <v>65</v>
       </c>
       <c r="G92" s="11" t="n">
-        <v>126153600</v>
+        <v>157692000</v>
       </c>
       <c r="H92" s="5" t="s">
         <v>22</v>
@@ -3659,7 +3659,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="7" t="s">
         <v>21</v>
       </c>
@@ -3677,7 +3677,7 @@
         <v>70</v>
       </c>
       <c r="G93" s="11" t="n">
-        <v>170315200</v>
+        <v>212894000</v>
       </c>
       <c r="H93" s="5" t="s">
         <v>22</v>
@@ -3695,7 +3695,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="7" t="s">
         <v>21</v>
       </c>
@@ -3713,7 +3713,7 @@
         <v>75</v>
       </c>
       <c r="G94" s="11" t="n">
-        <v>239173600</v>
+        <v>298967000</v>
       </c>
       <c r="H94" s="5" t="s">
         <v>22</v>
@@ -3731,7 +3731,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="7" t="s">
         <v>21</v>
       </c>
@@ -3749,7 +3749,7 @@
         <v>80</v>
       </c>
       <c r="G95" s="11" t="n">
-        <v>332695200</v>
+        <v>415869000</v>
       </c>
       <c r="H95" s="5" t="s">
         <v>22</v>
@@ -3767,7 +3767,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="7" t="s">
         <v>21</v>
       </c>
@@ -3785,7 +3785,7 @@
         <v>85</v>
       </c>
       <c r="G96" s="11" t="n">
-        <v>465772800</v>
+        <v>582216000</v>
       </c>
       <c r="H96" s="5" t="s">
         <v>22</v>
@@ -3803,7 +3803,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="7" t="s">
         <v>21</v>
       </c>
@@ -3821,7 +3821,7 @@
         <v>90</v>
       </c>
       <c r="G97" s="11" t="n">
-        <v>652081600</v>
+        <v>815102000</v>
       </c>
       <c r="H97" s="5" t="s">
         <v>22</v>
@@ -3839,7 +3839,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="7" t="s">
         <v>12</v>
       </c>
@@ -3857,7 +3857,7 @@
         <v>5</v>
       </c>
       <c r="G98" s="10" t="n">
-        <v>24893250</v>
+        <v>33191000</v>
       </c>
       <c r="H98" s="5" t="s">
         <v>23</v>
@@ -3875,7 +3875,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="7" t="s">
         <v>12</v>
       </c>
@@ -3893,7 +3893,7 @@
         <v>18</v>
       </c>
       <c r="G99" s="10" t="n">
-        <v>22333500</v>
+        <v>29778000</v>
       </c>
       <c r="H99" s="5" t="s">
         <v>23</v>
@@ -3911,7 +3911,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="7" t="s">
         <v>12</v>
       </c>
@@ -3929,7 +3929,7 @@
         <v>25</v>
       </c>
       <c r="G100" s="10" t="n">
-        <v>31683000</v>
+        <v>42244000</v>
       </c>
       <c r="H100" s="5" t="s">
         <v>23</v>
@@ -3947,7 +3947,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="7" t="s">
         <v>12</v>
       </c>
@@ -3965,7 +3965,7 @@
         <v>30</v>
       </c>
       <c r="G101" s="10" t="n">
-        <v>34080750</v>
+        <v>45441000</v>
       </c>
       <c r="H101" s="5" t="s">
         <v>23</v>
@@ -3983,7 +3983,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="7" t="s">
         <v>12</v>
       </c>
@@ -4001,7 +4001,7 @@
         <v>35</v>
       </c>
       <c r="G102" s="10" t="n">
-        <v>36531750</v>
+        <v>48709000</v>
       </c>
       <c r="H102" s="5" t="s">
         <v>23</v>
@@ -4019,7 +4019,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="7" t="s">
         <v>12</v>
       </c>
@@ -4037,7 +4037,7 @@
         <v>40</v>
       </c>
       <c r="G103" s="10" t="n">
-        <v>39049500</v>
+        <v>52066000</v>
       </c>
       <c r="H103" s="5" t="s">
         <v>23</v>
@@ -4055,7 +4055,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="7" t="s">
         <v>12</v>
       </c>
@@ -4073,7 +4073,7 @@
         <v>45</v>
       </c>
       <c r="G104" s="10" t="n">
-        <v>41613750</v>
+        <v>55485000</v>
       </c>
       <c r="H104" s="5" t="s">
         <v>23</v>
@@ -4091,7 +4091,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="7" t="s">
         <v>12</v>
       </c>
@@ -4109,7 +4109,7 @@
         <v>50</v>
       </c>
       <c r="G105" s="10" t="n">
-        <v>46650000</v>
+        <v>62200000</v>
       </c>
       <c r="H105" s="5" t="s">
         <v>23</v>
@@ -4127,7 +4127,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="7" t="s">
         <v>12</v>
       </c>
@@ -4145,7 +4145,7 @@
         <v>55</v>
       </c>
       <c r="G106" s="10" t="n">
-        <v>51783750</v>
+        <v>69045000</v>
       </c>
       <c r="H106" s="5" t="s">
         <v>23</v>
@@ -4163,7 +4163,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="7" t="s">
         <v>12</v>
       </c>
@@ -4181,7 +4181,7 @@
         <v>60</v>
       </c>
       <c r="G107" s="10" t="n">
-        <v>63775500</v>
+        <v>85034000</v>
       </c>
       <c r="H107" s="5" t="s">
         <v>23</v>
@@ -4199,7 +4199,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="7" t="s">
         <v>12</v>
       </c>
@@ -4217,7 +4217,7 @@
         <v>65</v>
       </c>
       <c r="G108" s="11" t="n">
-        <v>76536000</v>
+        <v>102048000</v>
       </c>
       <c r="H108" s="5" t="s">
         <v>23</v>
@@ -4235,7 +4235,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="7" t="s">
         <v>12</v>
       </c>
@@ -4253,7 +4253,7 @@
         <v>70</v>
       </c>
       <c r="G109" s="11" t="n">
-        <v>114829500</v>
+        <v>153106000</v>
       </c>
       <c r="H109" s="5" t="s">
         <v>23</v>
@@ -4271,7 +4271,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="7" t="s">
         <v>12</v>
       </c>
@@ -4289,7 +4289,7 @@
         <v>75</v>
       </c>
       <c r="G110" s="11" t="n">
-        <v>158478000</v>
+        <v>211304000</v>
       </c>
       <c r="H110" s="5" t="s">
         <v>23</v>
@@ -4307,7 +4307,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="7" t="s">
         <v>12</v>
       </c>
@@ -4325,7 +4325,7 @@
         <v>80</v>
       </c>
       <c r="G111" s="11" t="n">
-        <v>218670750</v>
+        <v>291561000</v>
       </c>
       <c r="H111" s="5" t="s">
         <v>23</v>
@@ -4343,7 +4343,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="7" t="s">
         <v>12</v>
       </c>
@@ -4361,7 +4361,7 @@
         <v>85</v>
       </c>
       <c r="G112" s="11" t="n">
-        <v>301744500</v>
+        <v>402326000</v>
       </c>
       <c r="H112" s="5" t="s">
         <v>23</v>
@@ -4379,7 +4379,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="7" t="s">
         <v>12</v>
       </c>
@@ -4397,7 +4397,7 @@
         <v>90</v>
       </c>
       <c r="G113" s="11" t="n">
-        <v>416389500</v>
+        <v>555186000</v>
       </c>
       <c r="H113" s="5" t="s">
         <v>23</v>
@@ -4415,7 +4415,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="7" t="s">
         <v>20</v>
       </c>
@@ -4433,7 +4433,7 @@
         <v>5</v>
       </c>
       <c r="G114" s="10" t="n">
-        <v>26649000</v>
+        <v>35532000</v>
       </c>
       <c r="H114" s="5" t="s">
         <v>23</v>
@@ -4451,7 +4451,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="7" t="s">
         <v>20</v>
       </c>
@@ -4469,7 +4469,7 @@
         <v>18</v>
       </c>
       <c r="G115" s="10" t="n">
-        <v>23169000</v>
+        <v>30892000</v>
       </c>
       <c r="H115" s="5" t="s">
         <v>23</v>
@@ -4487,7 +4487,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="7" t="s">
         <v>20</v>
       </c>
@@ -4505,7 +4505,7 @@
         <v>25</v>
       </c>
       <c r="G116" s="10" t="n">
-        <v>37731000</v>
+        <v>50308000</v>
       </c>
       <c r="H116" s="5" t="s">
         <v>23</v>
@@ -4523,7 +4523,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="7" t="s">
         <v>20</v>
       </c>
@@ -4541,7 +4541,7 @@
         <v>30</v>
       </c>
       <c r="G117" s="10" t="n">
-        <v>40560000</v>
+        <v>54080000</v>
       </c>
       <c r="H117" s="5" t="s">
         <v>23</v>
@@ -4559,7 +4559,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="7" t="s">
         <v>20</v>
       </c>
@@ -4577,7 +4577,7 @@
         <v>35</v>
       </c>
       <c r="G118" s="10" t="n">
-        <v>43389750</v>
+        <v>57853000</v>
       </c>
       <c r="H118" s="5" t="s">
         <v>23</v>
@@ -4595,7 +4595,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="7" t="s">
         <v>20</v>
       </c>
@@ -4613,7 +4613,7 @@
         <v>40</v>
       </c>
       <c r="G119" s="10" t="n">
-        <v>46385250</v>
+        <v>61847000</v>
       </c>
       <c r="H119" s="5" t="s">
         <v>23</v>
@@ -4631,7 +4631,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="7" t="s">
         <v>20</v>
       </c>
@@ -4649,7 +4649,7 @@
         <v>45</v>
       </c>
       <c r="G120" s="10" t="n">
-        <v>48715500</v>
+        <v>64954000</v>
       </c>
       <c r="H120" s="5" t="s">
         <v>23</v>
@@ -4667,7 +4667,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="7" t="s">
         <v>20</v>
       </c>
@@ -4685,7 +4685,7 @@
         <v>50</v>
       </c>
       <c r="G121" s="10" t="n">
-        <v>55116750</v>
+        <v>73489000</v>
       </c>
       <c r="H121" s="5" t="s">
         <v>23</v>
@@ -4703,7 +4703,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="7" t="s">
         <v>20</v>
       </c>
@@ -4721,7 +4721,7 @@
         <v>55</v>
       </c>
       <c r="G122" s="10" t="n">
-        <v>61787250</v>
+        <v>82383000</v>
       </c>
       <c r="H122" s="5" t="s">
         <v>23</v>
@@ -4739,7 +4739,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="7" t="s">
         <v>20</v>
       </c>
@@ -4757,7 +4757,7 @@
         <v>60</v>
       </c>
       <c r="G123" s="11" t="n">
-        <v>76053000</v>
+        <v>101404000</v>
       </c>
       <c r="H123" s="5" t="s">
         <v>23</v>
@@ -4775,7 +4775,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="7" t="s">
         <v>20</v>
       </c>
@@ -4793,7 +4793,7 @@
         <v>65</v>
       </c>
       <c r="G124" s="11" t="n">
-        <v>91263750</v>
+        <v>121685000</v>
       </c>
       <c r="H124" s="5" t="s">
         <v>23</v>
@@ -4811,7 +4811,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="7" t="s">
         <v>20</v>
       </c>
@@ -4829,7 +4829,7 @@
         <v>70</v>
       </c>
       <c r="G125" s="11" t="n">
-        <v>136880250</v>
+        <v>182507000</v>
       </c>
       <c r="H125" s="5" t="s">
         <v>23</v>
@@ -4847,7 +4847,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="7" t="s">
         <v>20</v>
       </c>
@@ -4865,7 +4865,7 @@
         <v>75</v>
       </c>
       <c r="G126" s="11" t="n">
-        <v>188923500</v>
+        <v>251898000</v>
       </c>
       <c r="H126" s="5" t="s">
         <v>23</v>
@@ -4883,7 +4883,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="7" t="s">
         <v>20</v>
       </c>
@@ -4901,7 +4901,7 @@
         <v>80</v>
       </c>
       <c r="G127" s="11" t="n">
-        <v>260730000</v>
+        <v>347640000</v>
       </c>
       <c r="H127" s="5" t="s">
         <v>23</v>
@@ -4919,7 +4919,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="7" t="s">
         <v>20</v>
       </c>
@@ -4937,7 +4937,7 @@
         <v>85</v>
       </c>
       <c r="G128" s="11" t="n">
-        <v>359812500</v>
+        <v>479750000</v>
       </c>
       <c r="H128" s="5" t="s">
         <v>23</v>
@@ -4955,7 +4955,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="7" t="s">
         <v>20</v>
       </c>
@@ -4973,7 +4973,7 @@
         <v>90</v>
       </c>
       <c r="G129" s="11" t="n">
-        <v>496521000</v>
+        <v>662028000</v>
       </c>
       <c r="H129" s="5" t="s">
         <v>23</v>
@@ -4991,7 +4991,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="7" t="s">
         <v>21</v>
       </c>
@@ -5009,7 +5009,7 @@
         <v>5</v>
       </c>
       <c r="G130" s="10" t="n">
-        <v>30513000</v>
+        <v>40684000</v>
       </c>
       <c r="H130" s="5" t="s">
         <v>23</v>
@@ -5027,7 +5027,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="7" t="s">
         <v>21</v>
       </c>
@@ -5045,7 +5045,7 @@
         <v>18</v>
       </c>
       <c r="G131" s="10" t="n">
-        <v>26527500</v>
+        <v>35370000</v>
       </c>
       <c r="H131" s="5" t="s">
         <v>23</v>
@@ -5063,7 +5063,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="7" t="s">
         <v>21</v>
       </c>
@@ -5081,7 +5081,7 @@
         <v>25</v>
       </c>
       <c r="G132" s="10" t="n">
-        <v>47754750</v>
+        <v>63673000</v>
       </c>
       <c r="H132" s="5" t="s">
         <v>23</v>
@@ -5099,7 +5099,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="7" t="s">
         <v>21</v>
       </c>
@@ -5117,7 +5117,7 @@
         <v>30</v>
       </c>
       <c r="G133" s="10" t="n">
-        <v>51160500</v>
+        <v>68214000</v>
       </c>
       <c r="H133" s="5" t="s">
         <v>23</v>
@@ -5135,7 +5135,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="7" t="s">
         <v>21</v>
       </c>
@@ -5153,7 +5153,7 @@
         <v>35</v>
       </c>
       <c r="G134" s="10" t="n">
-        <v>54613500</v>
+        <v>72818000</v>
       </c>
       <c r="H134" s="5" t="s">
         <v>23</v>
@@ -5171,7 +5171,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="7" t="s">
         <v>21</v>
       </c>
@@ -5189,7 +5189,7 @@
         <v>40</v>
       </c>
       <c r="G135" s="10" t="n">
-        <v>58029000</v>
+        <v>77372000</v>
       </c>
       <c r="H135" s="5" t="s">
         <v>23</v>
@@ -5207,7 +5207,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="7" t="s">
         <v>21</v>
       </c>
@@ -5225,7 +5225,7 @@
         <v>45</v>
       </c>
       <c r="G136" s="10" t="n">
-        <v>62577000</v>
+        <v>83436000</v>
       </c>
       <c r="H136" s="5" t="s">
         <v>23</v>
@@ -5243,7 +5243,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="7" t="s">
         <v>21</v>
       </c>
@@ -5261,7 +5261,7 @@
         <v>50</v>
       </c>
       <c r="G137" s="10" t="n">
-        <v>66080250</v>
+        <v>88107000</v>
       </c>
       <c r="H137" s="5" t="s">
         <v>23</v>
@@ -5279,7 +5279,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="7" t="s">
         <v>21</v>
       </c>
@@ -5297,7 +5297,7 @@
         <v>55</v>
       </c>
       <c r="G138" s="11" t="n">
-        <v>76006500</v>
+        <v>101342000</v>
       </c>
       <c r="H138" s="5" t="s">
         <v>23</v>
@@ -5315,7 +5315,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="7" t="s">
         <v>21</v>
       </c>
@@ -5333,7 +5333,7 @@
         <v>60</v>
       </c>
       <c r="G139" s="11" t="n">
-        <v>85527750</v>
+        <v>114037000</v>
       </c>
       <c r="H139" s="5" t="s">
         <v>23</v>
@@ -5351,7 +5351,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="7" t="s">
         <v>21</v>
       </c>
@@ -5369,7 +5369,7 @@
         <v>65</v>
       </c>
       <c r="G140" s="11" t="n">
-        <v>118269000</v>
+        <v>157692000</v>
       </c>
       <c r="H140" s="5" t="s">
         <v>23</v>
@@ -5387,7 +5387,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="7" t="s">
         <v>21</v>
       </c>
@@ -5405,7 +5405,7 @@
         <v>70</v>
       </c>
       <c r="G141" s="11" t="n">
-        <v>159670500</v>
+        <v>212894000</v>
       </c>
       <c r="H141" s="5" t="s">
         <v>23</v>
@@ -5423,7 +5423,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="7" t="s">
         <v>21</v>
       </c>
@@ -5441,7 +5441,7 @@
         <v>75</v>
       </c>
       <c r="G142" s="11" t="n">
-        <v>224225250</v>
+        <v>298967000</v>
       </c>
       <c r="H142" s="5" t="s">
         <v>23</v>
@@ -5459,7 +5459,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="7" t="s">
         <v>21</v>
       </c>
@@ -5477,7 +5477,7 @@
         <v>80</v>
       </c>
       <c r="G143" s="11" t="n">
-        <v>311901750</v>
+        <v>415869000</v>
       </c>
       <c r="H143" s="5" t="s">
         <v>23</v>
@@ -5495,7 +5495,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="7" t="s">
         <v>21</v>
       </c>
@@ -5513,7 +5513,7 @@
         <v>85</v>
       </c>
       <c r="G144" s="11" t="n">
-        <v>436662000</v>
+        <v>582216000</v>
       </c>
       <c r="H144" s="5" t="s">
         <v>23</v>
@@ -5531,7 +5531,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="7" t="s">
         <v>21</v>
       </c>
@@ -5549,7 +5549,7 @@
         <v>90</v>
       </c>
       <c r="G145" s="11" t="n">
-        <v>611326500</v>
+        <v>815102000</v>
       </c>
       <c r="H145" s="5" t="s">
         <v>23</v>
@@ -5567,7 +5567,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="7" t="s">
         <v>12</v>
       </c>
@@ -5585,7 +5585,7 @@
         <v>5</v>
       </c>
       <c r="G146" s="10" t="n">
-        <v>24893250</v>
+        <v>33191000</v>
       </c>
       <c r="H146" s="5" t="s">
         <v>15</v>
@@ -5603,7 +5603,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="7" t="s">
         <v>12</v>
       </c>
@@ -5621,7 +5621,7 @@
         <v>18</v>
       </c>
       <c r="G147" s="10" t="n">
-        <v>22333500</v>
+        <v>29778000</v>
       </c>
       <c r="H147" s="5" t="s">
         <v>15</v>
@@ -5639,7 +5639,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="7" t="s">
         <v>12</v>
       </c>
@@ -5657,7 +5657,7 @@
         <v>25</v>
       </c>
       <c r="G148" s="10" t="n">
-        <v>31683000</v>
+        <v>42244000</v>
       </c>
       <c r="H148" s="5" t="s">
         <v>15</v>
@@ -5675,7 +5675,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="7" t="s">
         <v>12</v>
       </c>
@@ -5693,7 +5693,7 @@
         <v>30</v>
       </c>
       <c r="G149" s="10" t="n">
-        <v>34080750</v>
+        <v>45441000</v>
       </c>
       <c r="H149" s="5" t="s">
         <v>15</v>
@@ -5711,7 +5711,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="7" t="s">
         <v>12</v>
       </c>
@@ -5729,7 +5729,7 @@
         <v>35</v>
       </c>
       <c r="G150" s="10" t="n">
-        <v>36531750</v>
+        <v>48709000</v>
       </c>
       <c r="H150" s="5" t="s">
         <v>15</v>
@@ -5747,7 +5747,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="7" t="s">
         <v>12</v>
       </c>
@@ -5765,7 +5765,7 @@
         <v>40</v>
       </c>
       <c r="G151" s="10" t="n">
-        <v>39049500</v>
+        <v>52066000</v>
       </c>
       <c r="H151" s="5" t="s">
         <v>15</v>
@@ -5783,7 +5783,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="7" t="s">
         <v>12</v>
       </c>
@@ -5801,7 +5801,7 @@
         <v>45</v>
       </c>
       <c r="G152" s="10" t="n">
-        <v>41613750</v>
+        <v>55485000</v>
       </c>
       <c r="H152" s="5" t="s">
         <v>15</v>
@@ -5819,7 +5819,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="7" t="s">
         <v>12</v>
       </c>
@@ -5837,7 +5837,7 @@
         <v>50</v>
       </c>
       <c r="G153" s="10" t="n">
-        <v>46650000</v>
+        <v>62200000</v>
       </c>
       <c r="H153" s="5" t="s">
         <v>15</v>
@@ -5855,7 +5855,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="7" t="s">
         <v>12</v>
       </c>
@@ -5873,7 +5873,7 @@
         <v>55</v>
       </c>
       <c r="G154" s="10" t="n">
-        <v>51783750</v>
+        <v>69045000</v>
       </c>
       <c r="H154" s="5" t="s">
         <v>15</v>
@@ -5891,7 +5891,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="7" t="s">
         <v>12</v>
       </c>
@@ -5909,7 +5909,7 @@
         <v>60</v>
       </c>
       <c r="G155" s="10" t="n">
-        <v>63775500</v>
+        <v>85034000</v>
       </c>
       <c r="H155" s="5" t="s">
         <v>15</v>
@@ -5927,7 +5927,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="7" t="s">
         <v>12</v>
       </c>
@@ -5945,7 +5945,7 @@
         <v>65</v>
       </c>
       <c r="G156" s="11" t="n">
-        <v>76536000</v>
+        <v>102048000</v>
       </c>
       <c r="H156" s="5" t="s">
         <v>15</v>
@@ -5963,7 +5963,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="7" t="s">
         <v>12</v>
       </c>
@@ -5981,7 +5981,7 @@
         <v>70</v>
       </c>
       <c r="G157" s="11" t="n">
-        <v>114829500</v>
+        <v>153106000</v>
       </c>
       <c r="H157" s="5" t="s">
         <v>15</v>
@@ -5999,7 +5999,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="7" t="s">
         <v>12</v>
       </c>
@@ -6017,7 +6017,7 @@
         <v>75</v>
       </c>
       <c r="G158" s="11" t="n">
-        <v>158478000</v>
+        <v>211304000</v>
       </c>
       <c r="H158" s="5" t="s">
         <v>15</v>
@@ -6035,7 +6035,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="7" t="s">
         <v>12</v>
       </c>
@@ -6053,7 +6053,7 @@
         <v>80</v>
       </c>
       <c r="G159" s="11" t="n">
-        <v>218670750</v>
+        <v>291561000</v>
       </c>
       <c r="H159" s="5" t="s">
         <v>15</v>
@@ -6071,7 +6071,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="7" t="s">
         <v>12</v>
       </c>
@@ -6089,7 +6089,7 @@
         <v>85</v>
       </c>
       <c r="G160" s="11" t="n">
-        <v>301744500</v>
+        <v>402326000</v>
       </c>
       <c r="H160" s="5" t="s">
         <v>15</v>
@@ -6107,7 +6107,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="7" t="s">
         <v>12</v>
       </c>
@@ -6125,7 +6125,7 @@
         <v>90</v>
       </c>
       <c r="G161" s="11" t="n">
-        <v>416389500</v>
+        <v>555186000</v>
       </c>
       <c r="H161" s="5" t="s">
         <v>15</v>
@@ -6143,7 +6143,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="7" t="s">
         <v>20</v>
       </c>
@@ -6161,7 +6161,7 @@
         <v>5</v>
       </c>
       <c r="G162" s="10" t="n">
-        <v>26649000</v>
+        <v>35532000</v>
       </c>
       <c r="H162" s="5" t="s">
         <v>15</v>
@@ -6179,7 +6179,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="7" t="s">
         <v>20</v>
       </c>
@@ -6197,7 +6197,7 @@
         <v>18</v>
       </c>
       <c r="G163" s="10" t="n">
-        <v>23169000</v>
+        <v>30892000</v>
       </c>
       <c r="H163" s="5" t="s">
         <v>15</v>
@@ -6215,7 +6215,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="7" t="s">
         <v>20</v>
       </c>
@@ -6233,7 +6233,7 @@
         <v>25</v>
       </c>
       <c r="G164" s="10" t="n">
-        <v>37731000</v>
+        <v>50308000</v>
       </c>
       <c r="H164" s="5" t="s">
         <v>15</v>
@@ -6251,7 +6251,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="7" t="s">
         <v>20</v>
       </c>
@@ -6269,7 +6269,7 @@
         <v>30</v>
       </c>
       <c r="G165" s="10" t="n">
-        <v>40560000</v>
+        <v>54080000</v>
       </c>
       <c r="H165" s="5" t="s">
         <v>15</v>
@@ -6287,7 +6287,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="7" t="s">
         <v>20</v>
       </c>
@@ -6305,7 +6305,7 @@
         <v>35</v>
       </c>
       <c r="G166" s="10" t="n">
-        <v>43389750</v>
+        <v>57853000</v>
       </c>
       <c r="H166" s="5" t="s">
         <v>15</v>
@@ -6323,7 +6323,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="7" t="s">
         <v>20</v>
       </c>
@@ -6341,7 +6341,7 @@
         <v>40</v>
       </c>
       <c r="G167" s="10" t="n">
-        <v>46385250</v>
+        <v>61847000</v>
       </c>
       <c r="H167" s="5" t="s">
         <v>15</v>
@@ -6359,7 +6359,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="7" t="s">
         <v>20</v>
       </c>
@@ -6377,7 +6377,7 @@
         <v>45</v>
       </c>
       <c r="G168" s="10" t="n">
-        <v>48715500</v>
+        <v>64954000</v>
       </c>
       <c r="H168" s="5" t="s">
         <v>15</v>
@@ -6395,7 +6395,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="7" t="s">
         <v>20</v>
       </c>
@@ -6413,7 +6413,7 @@
         <v>50</v>
       </c>
       <c r="G169" s="10" t="n">
-        <v>55116750</v>
+        <v>73489000</v>
       </c>
       <c r="H169" s="5" t="s">
         <v>15</v>
@@ -6431,7 +6431,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="7" t="s">
         <v>20</v>
       </c>
@@ -6449,7 +6449,7 @@
         <v>55</v>
       </c>
       <c r="G170" s="10" t="n">
-        <v>61787250</v>
+        <v>82383000</v>
       </c>
       <c r="H170" s="5" t="s">
         <v>15</v>
@@ -6467,7 +6467,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="7" t="s">
         <v>20</v>
       </c>
@@ -6485,7 +6485,7 @@
         <v>60</v>
       </c>
       <c r="G171" s="11" t="n">
-        <v>76053000</v>
+        <v>101404000</v>
       </c>
       <c r="H171" s="5" t="s">
         <v>15</v>
@@ -6503,7 +6503,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="7" t="s">
         <v>20</v>
       </c>
@@ -6521,7 +6521,7 @@
         <v>65</v>
       </c>
       <c r="G172" s="11" t="n">
-        <v>91263750</v>
+        <v>121685000</v>
       </c>
       <c r="H172" s="5" t="s">
         <v>15</v>
@@ -6539,7 +6539,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="7" t="s">
         <v>20</v>
       </c>
@@ -6557,7 +6557,7 @@
         <v>70</v>
       </c>
       <c r="G173" s="11" t="n">
-        <v>136880250</v>
+        <v>182507000</v>
       </c>
       <c r="H173" s="5" t="s">
         <v>15</v>
@@ -6575,7 +6575,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="7" t="s">
         <v>20</v>
       </c>
@@ -6593,7 +6593,7 @@
         <v>75</v>
       </c>
       <c r="G174" s="11" t="n">
-        <v>188923500</v>
+        <v>251898000</v>
       </c>
       <c r="H174" s="5" t="s">
         <v>15</v>
@@ -6611,7 +6611,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="7" t="s">
         <v>20</v>
       </c>
@@ -6629,7 +6629,7 @@
         <v>80</v>
       </c>
       <c r="G175" s="11" t="n">
-        <v>260730000</v>
+        <v>347640000</v>
       </c>
       <c r="H175" s="5" t="s">
         <v>15</v>
@@ -6647,7 +6647,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="7" t="s">
         <v>20</v>
       </c>
@@ -6665,7 +6665,7 @@
         <v>85</v>
       </c>
       <c r="G176" s="11" t="n">
-        <v>359812500</v>
+        <v>479750000</v>
       </c>
       <c r="H176" s="5" t="s">
         <v>15</v>
@@ -6683,7 +6683,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="177" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="7" t="s">
         <v>20</v>
       </c>
@@ -6701,7 +6701,7 @@
         <v>90</v>
       </c>
       <c r="G177" s="11" t="n">
-        <v>496521000</v>
+        <v>662028000</v>
       </c>
       <c r="H177" s="5" t="s">
         <v>15</v>
@@ -6719,7 +6719,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="7" t="s">
         <v>21</v>
       </c>
@@ -6737,7 +6737,7 @@
         <v>5</v>
       </c>
       <c r="G178" s="10" t="n">
-        <v>30513000</v>
+        <v>40684000</v>
       </c>
       <c r="H178" s="5" t="s">
         <v>15</v>
@@ -6755,7 +6755,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="7" t="s">
         <v>21</v>
       </c>
@@ -6773,7 +6773,7 @@
         <v>18</v>
       </c>
       <c r="G179" s="10" t="n">
-        <v>26527500</v>
+        <v>35370000</v>
       </c>
       <c r="H179" s="5" t="s">
         <v>15</v>
@@ -6791,7 +6791,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="7" t="s">
         <v>21</v>
       </c>
@@ -6809,7 +6809,7 @@
         <v>25</v>
       </c>
       <c r="G180" s="10" t="n">
-        <v>47754750</v>
+        <v>63673000</v>
       </c>
       <c r="H180" s="5" t="s">
         <v>15</v>
@@ -6827,7 +6827,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="7" t="s">
         <v>21</v>
       </c>
@@ -6845,7 +6845,7 @@
         <v>30</v>
       </c>
       <c r="G181" s="10" t="n">
-        <v>51160500</v>
+        <v>68214000</v>
       </c>
       <c r="H181" s="5" t="s">
         <v>15</v>
@@ -6863,7 +6863,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="7" t="s">
         <v>21</v>
       </c>
@@ -6881,7 +6881,7 @@
         <v>35</v>
       </c>
       <c r="G182" s="10" t="n">
-        <v>54613500</v>
+        <v>72818000</v>
       </c>
       <c r="H182" s="5" t="s">
         <v>15</v>
@@ -6899,7 +6899,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="183" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="183" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="7" t="s">
         <v>21</v>
       </c>
@@ -6917,7 +6917,7 @@
         <v>40</v>
       </c>
       <c r="G183" s="10" t="n">
-        <v>58029000</v>
+        <v>77372000</v>
       </c>
       <c r="H183" s="5" t="s">
         <v>15</v>
@@ -6935,7 +6935,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="184" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="7" t="s">
         <v>21</v>
       </c>
@@ -6953,7 +6953,7 @@
         <v>45</v>
       </c>
       <c r="G184" s="10" t="n">
-        <v>62577000</v>
+        <v>83436000</v>
       </c>
       <c r="H184" s="5" t="s">
         <v>15</v>
@@ -6971,7 +6971,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="7" t="s">
         <v>21</v>
       </c>
@@ -6989,7 +6989,7 @@
         <v>50</v>
       </c>
       <c r="G185" s="10" t="n">
-        <v>66080250</v>
+        <v>88107000</v>
       </c>
       <c r="H185" s="5" t="s">
         <v>15</v>
@@ -7007,7 +7007,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="186" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="7" t="s">
         <v>21</v>
       </c>
@@ -7025,7 +7025,7 @@
         <v>55</v>
       </c>
       <c r="G186" s="11" t="n">
-        <v>76006500</v>
+        <v>101342000</v>
       </c>
       <c r="H186" s="5" t="s">
         <v>15</v>
@@ -7043,7 +7043,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="187" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="187" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="7" t="s">
         <v>21</v>
       </c>
@@ -7061,7 +7061,7 @@
         <v>60</v>
       </c>
       <c r="G187" s="11" t="n">
-        <v>85527750</v>
+        <v>114037000</v>
       </c>
       <c r="H187" s="5" t="s">
         <v>15</v>
@@ -7079,7 +7079,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="188" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="188" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="7" t="s">
         <v>21</v>
       </c>
@@ -7097,7 +7097,7 @@
         <v>65</v>
       </c>
       <c r="G188" s="11" t="n">
-        <v>118269000</v>
+        <v>157692000</v>
       </c>
       <c r="H188" s="5" t="s">
         <v>15</v>
@@ -7115,7 +7115,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="189" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="189" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="7" t="s">
         <v>21</v>
       </c>
@@ -7133,7 +7133,7 @@
         <v>70</v>
       </c>
       <c r="G189" s="11" t="n">
-        <v>159670500</v>
+        <v>212894000</v>
       </c>
       <c r="H189" s="5" t="s">
         <v>15</v>
@@ -7151,7 +7151,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="190" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="190" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="7" t="s">
         <v>21</v>
       </c>
@@ -7169,7 +7169,7 @@
         <v>75</v>
       </c>
       <c r="G190" s="11" t="n">
-        <v>224225250</v>
+        <v>298967000</v>
       </c>
       <c r="H190" s="5" t="s">
         <v>15</v>
@@ -7187,7 +7187,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="191" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="191" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="7" t="s">
         <v>21</v>
       </c>
@@ -7205,7 +7205,7 @@
         <v>80</v>
       </c>
       <c r="G191" s="11" t="n">
-        <v>311901750</v>
+        <v>415869000</v>
       </c>
       <c r="H191" s="5" t="s">
         <v>15</v>
@@ -7223,7 +7223,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="192" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="192" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="7" t="s">
         <v>21</v>
       </c>
@@ -7241,7 +7241,7 @@
         <v>85</v>
       </c>
       <c r="G192" s="11" t="n">
-        <v>436662000</v>
+        <v>582216000</v>
       </c>
       <c r="H192" s="5" t="s">
         <v>15</v>
@@ -7259,7 +7259,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="193" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="193" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="7" t="s">
         <v>21</v>
       </c>
@@ -7277,7 +7277,7 @@
         <v>90</v>
       </c>
       <c r="G193" s="11" t="n">
-        <v>611326500</v>
+        <v>815102000</v>
       </c>
       <c r="H193" s="5" t="s">
         <v>15</v>
@@ -7295,7 +7295,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="194" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="194" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="7" t="s">
         <v>12</v>
       </c>
@@ -7313,7 +7313,7 @@
         <v>5</v>
       </c>
       <c r="G194" s="10" t="n">
-        <v>19914600</v>
+        <v>33191000</v>
       </c>
       <c r="H194" s="5" t="s">
         <v>22</v>
@@ -7331,7 +7331,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="195" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="195" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="7" t="s">
         <v>12</v>
       </c>
@@ -7349,7 +7349,7 @@
         <v>18</v>
       </c>
       <c r="G195" s="10" t="n">
-        <v>17866800</v>
+        <v>29778000</v>
       </c>
       <c r="H195" s="5" t="s">
         <v>22</v>
@@ -7367,7 +7367,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="196" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="196" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="7" t="s">
         <v>12</v>
       </c>
@@ -7385,7 +7385,7 @@
         <v>25</v>
       </c>
       <c r="G196" s="10" t="n">
-        <v>25346400</v>
+        <v>42244000</v>
       </c>
       <c r="H196" s="5" t="s">
         <v>22</v>
@@ -7403,7 +7403,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="197" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="197" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="7" t="s">
         <v>12</v>
       </c>
@@ -7421,7 +7421,7 @@
         <v>30</v>
       </c>
       <c r="G197" s="10" t="n">
-        <v>27264600</v>
+        <v>45441000</v>
       </c>
       <c r="H197" s="5" t="s">
         <v>22</v>
@@ -7439,7 +7439,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="198" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="198" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="7" t="s">
         <v>12</v>
       </c>
@@ -7457,7 +7457,7 @@
         <v>35</v>
       </c>
       <c r="G198" s="10" t="n">
-        <v>29225400</v>
+        <v>48709000</v>
       </c>
       <c r="H198" s="5" t="s">
         <v>22</v>
@@ -7475,7 +7475,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="199" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="199" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="7" t="s">
         <v>12</v>
       </c>
@@ -7493,7 +7493,7 @@
         <v>40</v>
       </c>
       <c r="G199" s="10" t="n">
-        <v>31239600</v>
+        <v>52066000</v>
       </c>
       <c r="H199" s="5" t="s">
         <v>22</v>
@@ -7511,7 +7511,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="200" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="200" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="7" t="s">
         <v>12</v>
       </c>
@@ -7529,7 +7529,7 @@
         <v>45</v>
       </c>
       <c r="G200" s="10" t="n">
-        <v>33291000</v>
+        <v>55485000</v>
       </c>
       <c r="H200" s="5" t="s">
         <v>22</v>
@@ -7547,7 +7547,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="201" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="201" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="7" t="s">
         <v>12</v>
       </c>
@@ -7565,7 +7565,7 @@
         <v>50</v>
       </c>
       <c r="G201" s="10" t="n">
-        <v>37320000</v>
+        <v>62200000</v>
       </c>
       <c r="H201" s="5" t="s">
         <v>22</v>
@@ -7583,7 +7583,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="202" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="202" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="7" t="s">
         <v>12</v>
       </c>
@@ -7601,7 +7601,7 @@
         <v>55</v>
       </c>
       <c r="G202" s="10" t="n">
-        <v>41427000</v>
+        <v>69045000</v>
       </c>
       <c r="H202" s="5" t="s">
         <v>22</v>
@@ -7619,7 +7619,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="203" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="203" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="7" t="s">
         <v>12</v>
       </c>
@@ -7637,7 +7637,7 @@
         <v>60</v>
       </c>
       <c r="G203" s="10" t="n">
-        <v>51020400</v>
+        <v>85034000</v>
       </c>
       <c r="H203" s="5" t="s">
         <v>22</v>
@@ -7655,7 +7655,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="204" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="204" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="7" t="s">
         <v>12</v>
       </c>
@@ -7673,7 +7673,7 @@
         <v>65</v>
       </c>
       <c r="G204" s="11" t="n">
-        <v>61228800</v>
+        <v>102048000</v>
       </c>
       <c r="H204" s="5" t="s">
         <v>22</v>
@@ -7691,7 +7691,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="205" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="205" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="7" t="s">
         <v>12</v>
       </c>
@@ -7709,7 +7709,7 @@
         <v>70</v>
       </c>
       <c r="G205" s="11" t="n">
-        <v>91863600</v>
+        <v>153106000</v>
       </c>
       <c r="H205" s="5" t="s">
         <v>22</v>
@@ -7727,7 +7727,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="206" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="206" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="7" t="s">
         <v>12</v>
       </c>
@@ -7745,7 +7745,7 @@
         <v>75</v>
       </c>
       <c r="G206" s="11" t="n">
-        <v>126782400</v>
+        <v>211304000</v>
       </c>
       <c r="H206" s="5" t="s">
         <v>22</v>
@@ -7763,7 +7763,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="207" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="207" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="7" t="s">
         <v>12</v>
       </c>
@@ -7781,7 +7781,7 @@
         <v>80</v>
       </c>
       <c r="G207" s="11" t="n">
-        <v>174936600</v>
+        <v>291561000</v>
       </c>
       <c r="H207" s="5" t="s">
         <v>22</v>
@@ -7799,7 +7799,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="208" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="208" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="7" t="s">
         <v>12</v>
       </c>
@@ -7817,7 +7817,7 @@
         <v>85</v>
       </c>
       <c r="G208" s="11" t="n">
-        <v>241395600</v>
+        <v>402326000</v>
       </c>
       <c r="H208" s="5" t="s">
         <v>22</v>
@@ -7835,7 +7835,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="209" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="209" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="7" t="s">
         <v>12</v>
       </c>
@@ -7853,7 +7853,7 @@
         <v>90</v>
       </c>
       <c r="G209" s="11" t="n">
-        <v>333111600</v>
+        <v>555186000</v>
       </c>
       <c r="H209" s="5" t="s">
         <v>22</v>
@@ -7871,7 +7871,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="210" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="210" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="7" t="s">
         <v>20</v>
       </c>
@@ -7889,7 +7889,7 @@
         <v>5</v>
       </c>
       <c r="G210" s="10" t="n">
-        <v>21319200</v>
+        <v>35532000</v>
       </c>
       <c r="H210" s="5" t="s">
         <v>22</v>
@@ -7907,7 +7907,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="211" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="211" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="7" t="s">
         <v>20</v>
       </c>
@@ -7925,7 +7925,7 @@
         <v>18</v>
       </c>
       <c r="G211" s="10" t="n">
-        <v>18535200</v>
+        <v>30892000</v>
       </c>
       <c r="H211" s="5" t="s">
         <v>22</v>
@@ -7943,7 +7943,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="212" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="212" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="7" t="s">
         <v>20</v>
       </c>
@@ -7961,7 +7961,7 @@
         <v>25</v>
       </c>
       <c r="G212" s="10" t="n">
-        <v>30184800</v>
+        <v>50308000</v>
       </c>
       <c r="H212" s="5" t="s">
         <v>22</v>
@@ -7979,7 +7979,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="213" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="213" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="7" t="s">
         <v>20</v>
       </c>
@@ -7997,7 +7997,7 @@
         <v>30</v>
       </c>
       <c r="G213" s="10" t="n">
-        <v>32448000</v>
+        <v>54080000</v>
       </c>
       <c r="H213" s="5" t="s">
         <v>22</v>
@@ -8015,7 +8015,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="214" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="214" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="7" t="s">
         <v>20</v>
       </c>
@@ -8033,7 +8033,7 @@
         <v>35</v>
       </c>
       <c r="G214" s="10" t="n">
-        <v>34711800</v>
+        <v>57853000</v>
       </c>
       <c r="H214" s="5" t="s">
         <v>22</v>
@@ -8051,7 +8051,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="215" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="215" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="7" t="s">
         <v>20</v>
       </c>
@@ -8069,7 +8069,7 @@
         <v>40</v>
       </c>
       <c r="G215" s="10" t="n">
-        <v>37108200</v>
+        <v>61847000</v>
       </c>
       <c r="H215" s="5" t="s">
         <v>22</v>
@@ -8087,7 +8087,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="216" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="216" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="7" t="s">
         <v>20</v>
       </c>
@@ -8105,7 +8105,7 @@
         <v>45</v>
       </c>
       <c r="G216" s="10" t="n">
-        <v>38972400</v>
+        <v>64954000</v>
       </c>
       <c r="H216" s="5" t="s">
         <v>22</v>
@@ -8123,7 +8123,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="217" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="217" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="7" t="s">
         <v>20</v>
       </c>
@@ -8141,7 +8141,7 @@
         <v>50</v>
       </c>
       <c r="G217" s="10" t="n">
-        <v>44093400</v>
+        <v>73489000</v>
       </c>
       <c r="H217" s="5" t="s">
         <v>22</v>
@@ -8159,7 +8159,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="218" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="218" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="7" t="s">
         <v>20</v>
       </c>
@@ -8177,7 +8177,7 @@
         <v>55</v>
       </c>
       <c r="G218" s="10" t="n">
-        <v>49429800</v>
+        <v>82383000</v>
       </c>
       <c r="H218" s="5" t="s">
         <v>22</v>
@@ -8195,7 +8195,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="219" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="219" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="7" t="s">
         <v>20</v>
       </c>
@@ -8213,7 +8213,7 @@
         <v>60</v>
       </c>
       <c r="G219" s="11" t="n">
-        <v>60842400</v>
+        <v>101404000</v>
       </c>
       <c r="H219" s="5" t="s">
         <v>22</v>
@@ -8231,7 +8231,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="220" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="220" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="7" t="s">
         <v>20</v>
       </c>
@@ -8249,7 +8249,7 @@
         <v>65</v>
       </c>
       <c r="G220" s="11" t="n">
-        <v>73011000</v>
+        <v>121685000</v>
       </c>
       <c r="H220" s="5" t="s">
         <v>22</v>
@@ -8267,7 +8267,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="221" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="221" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="7" t="s">
         <v>20</v>
       </c>
@@ -8285,7 +8285,7 @@
         <v>70</v>
       </c>
       <c r="G221" s="11" t="n">
-        <v>109504200</v>
+        <v>182507000</v>
       </c>
       <c r="H221" s="5" t="s">
         <v>22</v>
@@ -8303,7 +8303,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="222" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="222" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="7" t="s">
         <v>20</v>
       </c>
@@ -8321,7 +8321,7 @@
         <v>75</v>
       </c>
       <c r="G222" s="11" t="n">
-        <v>151138800</v>
+        <v>251898000</v>
       </c>
       <c r="H222" s="5" t="s">
         <v>22</v>
@@ -8339,7 +8339,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="223" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="223" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="7" t="s">
         <v>20</v>
       </c>
@@ -8357,7 +8357,7 @@
         <v>80</v>
       </c>
       <c r="G223" s="11" t="n">
-        <v>208584000</v>
+        <v>347640000</v>
       </c>
       <c r="H223" s="5" t="s">
         <v>22</v>
@@ -8375,7 +8375,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="224" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="224" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="7" t="s">
         <v>20</v>
       </c>
@@ -8393,7 +8393,7 @@
         <v>85</v>
       </c>
       <c r="G224" s="11" t="n">
-        <v>287850000</v>
+        <v>479750000</v>
       </c>
       <c r="H224" s="5" t="s">
         <v>22</v>
@@ -8411,7 +8411,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="225" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="225" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="7" t="s">
         <v>20</v>
       </c>
@@ -8429,7 +8429,7 @@
         <v>90</v>
       </c>
       <c r="G225" s="11" t="n">
-        <v>397216800</v>
+        <v>662028000</v>
       </c>
       <c r="H225" s="5" t="s">
         <v>22</v>
@@ -8447,7 +8447,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="226" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="226" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="7" t="s">
         <v>21</v>
       </c>
@@ -8465,7 +8465,7 @@
         <v>5</v>
       </c>
       <c r="G226" s="10" t="n">
-        <v>24410400</v>
+        <v>40684000</v>
       </c>
       <c r="H226" s="5" t="s">
         <v>22</v>
@@ -8483,7 +8483,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="227" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="227" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="7" t="s">
         <v>21</v>
       </c>
@@ -8501,7 +8501,7 @@
         <v>18</v>
       </c>
       <c r="G227" s="10" t="n">
-        <v>21222000</v>
+        <v>35370000</v>
       </c>
       <c r="H227" s="5" t="s">
         <v>22</v>
@@ -8519,7 +8519,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="228" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="228" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="7" t="s">
         <v>21</v>
       </c>
@@ -8537,7 +8537,7 @@
         <v>25</v>
       </c>
       <c r="G228" s="10" t="n">
-        <v>38203800</v>
+        <v>63673000</v>
       </c>
       <c r="H228" s="5" t="s">
         <v>22</v>
@@ -8555,7 +8555,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="229" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="229" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="7" t="s">
         <v>21</v>
       </c>
@@ -8573,7 +8573,7 @@
         <v>30</v>
       </c>
       <c r="G229" s="10" t="n">
-        <v>40928400</v>
+        <v>68214000</v>
       </c>
       <c r="H229" s="5" t="s">
         <v>22</v>
@@ -8591,7 +8591,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="230" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="230" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="7" t="s">
         <v>21</v>
       </c>
@@ -8609,7 +8609,7 @@
         <v>35</v>
       </c>
       <c r="G230" s="10" t="n">
-        <v>43690800</v>
+        <v>72818000</v>
       </c>
       <c r="H230" s="5" t="s">
         <v>22</v>
@@ -8627,7 +8627,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="231" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="231" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="7" t="s">
         <v>21</v>
       </c>
@@ -8645,7 +8645,7 @@
         <v>40</v>
       </c>
       <c r="G231" s="10" t="n">
-        <v>46423200</v>
+        <v>77372000</v>
       </c>
       <c r="H231" s="5" t="s">
         <v>22</v>
@@ -8663,7 +8663,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="232" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="232" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="7" t="s">
         <v>21</v>
       </c>
@@ -8681,7 +8681,7 @@
         <v>45</v>
       </c>
       <c r="G232" s="10" t="n">
-        <v>50061600</v>
+        <v>83436000</v>
       </c>
       <c r="H232" s="5" t="s">
         <v>22</v>
@@ -8699,7 +8699,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="233" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="233" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="7" t="s">
         <v>21</v>
       </c>
@@ -8717,7 +8717,7 @@
         <v>50</v>
       </c>
       <c r="G233" s="10" t="n">
-        <v>52864200</v>
+        <v>88107000</v>
       </c>
       <c r="H233" s="5" t="s">
         <v>22</v>
@@ -8735,7 +8735,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="234" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="234" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="7" t="s">
         <v>21</v>
       </c>
@@ -8753,7 +8753,7 @@
         <v>55</v>
       </c>
       <c r="G234" s="11" t="n">
-        <v>60805200</v>
+        <v>101342000</v>
       </c>
       <c r="H234" s="5" t="s">
         <v>22</v>
@@ -8771,7 +8771,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="235" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="235" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="7" t="s">
         <v>21</v>
       </c>
@@ -8789,7 +8789,7 @@
         <v>60</v>
       </c>
       <c r="G235" s="11" t="n">
-        <v>68422200</v>
+        <v>114037000</v>
       </c>
       <c r="H235" s="5" t="s">
         <v>22</v>
@@ -8807,7 +8807,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="236" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="236" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="7" t="s">
         <v>21</v>
       </c>
@@ -8825,7 +8825,7 @@
         <v>65</v>
       </c>
       <c r="G236" s="11" t="n">
-        <v>94615200</v>
+        <v>157692000</v>
       </c>
       <c r="H236" s="5" t="s">
         <v>22</v>
@@ -8843,7 +8843,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="237" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="237" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="7" t="s">
         <v>21</v>
       </c>
@@ -8861,7 +8861,7 @@
         <v>70</v>
       </c>
       <c r="G237" s="11" t="n">
-        <v>127736400</v>
+        <v>212894000</v>
       </c>
       <c r="H237" s="5" t="s">
         <v>22</v>
@@ -8879,7 +8879,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="238" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="238" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="7" t="s">
         <v>21</v>
       </c>
@@ -8897,7 +8897,7 @@
         <v>75</v>
       </c>
       <c r="G238" s="11" t="n">
-        <v>179380200</v>
+        <v>298967000</v>
       </c>
       <c r="H238" s="5" t="s">
         <v>22</v>
@@ -8915,7 +8915,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="239" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="239" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="7" t="s">
         <v>21</v>
       </c>
@@ -8933,7 +8933,7 @@
         <v>80</v>
       </c>
       <c r="G239" s="11" t="n">
-        <v>249521400</v>
+        <v>415869000</v>
       </c>
       <c r="H239" s="5" t="s">
         <v>22</v>
@@ -8951,7 +8951,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="240" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="240" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="7" t="s">
         <v>21</v>
       </c>
@@ -8969,7 +8969,7 @@
         <v>85</v>
       </c>
       <c r="G240" s="11" t="n">
-        <v>349329600</v>
+        <v>582216000</v>
       </c>
       <c r="H240" s="5" t="s">
         <v>22</v>
@@ -8987,7 +8987,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="241" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="241" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="7" t="s">
         <v>21</v>
       </c>
@@ -9005,7 +9005,7 @@
         <v>90</v>
       </c>
       <c r="G241" s="11" t="n">
-        <v>489061200</v>
+        <v>815102000</v>
       </c>
       <c r="H241" s="5" t="s">
         <v>22</v>
@@ -9023,7 +9023,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="242" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="242" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="7" t="s">
         <v>12</v>
       </c>
@@ -9041,7 +9041,7 @@
         <v>5</v>
       </c>
       <c r="G242" s="10" t="n">
-        <v>18669937.5</v>
+        <v>33191000</v>
       </c>
       <c r="H242" s="5" t="s">
         <v>23</v>
@@ -9059,7 +9059,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="243" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="243" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="7" t="s">
         <v>12</v>
       </c>
@@ -9077,7 +9077,7 @@
         <v>18</v>
       </c>
       <c r="G243" s="10" t="n">
-        <v>16750125</v>
+        <v>29778000</v>
       </c>
       <c r="H243" s="5" t="s">
         <v>23</v>
@@ -9095,7 +9095,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="244" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="244" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="7" t="s">
         <v>12</v>
       </c>
@@ -9113,7 +9113,7 @@
         <v>25</v>
       </c>
       <c r="G244" s="10" t="n">
-        <v>23762250</v>
+        <v>42244000</v>
       </c>
       <c r="H244" s="5" t="s">
         <v>23</v>
@@ -9131,7 +9131,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="245" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="245" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="7" t="s">
         <v>12</v>
       </c>
@@ -9149,7 +9149,7 @@
         <v>30</v>
       </c>
       <c r="G245" s="10" t="n">
-        <v>25560562.5</v>
+        <v>45441000</v>
       </c>
       <c r="H245" s="5" t="s">
         <v>23</v>
@@ -9167,7 +9167,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="246" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="246" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="7" t="s">
         <v>12</v>
       </c>
@@ -9185,7 +9185,7 @@
         <v>35</v>
       </c>
       <c r="G246" s="10" t="n">
-        <v>27398812.5</v>
+        <v>48709000</v>
       </c>
       <c r="H246" s="5" t="s">
         <v>23</v>
@@ -9203,7 +9203,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="247" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="247" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="7" t="s">
         <v>12</v>
       </c>
@@ -9221,7 +9221,7 @@
         <v>40</v>
       </c>
       <c r="G247" s="10" t="n">
-        <v>29287125</v>
+        <v>52066000</v>
       </c>
       <c r="H247" s="5" t="s">
         <v>23</v>
@@ -9239,7 +9239,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="248" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="248" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="7" t="s">
         <v>12</v>
       </c>
@@ -9257,7 +9257,7 @@
         <v>45</v>
       </c>
       <c r="G248" s="10" t="n">
-        <v>31210312.5</v>
+        <v>55485000</v>
       </c>
       <c r="H248" s="5" t="s">
         <v>23</v>
@@ -9275,7 +9275,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="249" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="249" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="7" t="s">
         <v>12</v>
       </c>
@@ -9293,7 +9293,7 @@
         <v>50</v>
       </c>
       <c r="G249" s="10" t="n">
-        <v>34987500</v>
+        <v>62200000</v>
       </c>
       <c r="H249" s="5" t="s">
         <v>23</v>
@@ -9311,7 +9311,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="250" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="250" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="7" t="s">
         <v>12</v>
       </c>
@@ -9329,7 +9329,7 @@
         <v>55</v>
       </c>
       <c r="G250" s="10" t="n">
-        <v>38837812.5</v>
+        <v>69045000</v>
       </c>
       <c r="H250" s="5" t="s">
         <v>23</v>
@@ -9347,7 +9347,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="251" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="251" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="7" t="s">
         <v>12</v>
       </c>
@@ -9365,7 +9365,7 @@
         <v>60</v>
       </c>
       <c r="G251" s="10" t="n">
-        <v>47831625</v>
+        <v>85034000</v>
       </c>
       <c r="H251" s="5" t="s">
         <v>23</v>
@@ -9383,7 +9383,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="252" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="252" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="7" t="s">
         <v>12</v>
       </c>
@@ -9401,7 +9401,7 @@
         <v>65</v>
       </c>
       <c r="G252" s="11" t="n">
-        <v>57402000</v>
+        <v>102048000</v>
       </c>
       <c r="H252" s="5" t="s">
         <v>23</v>
@@ -9419,7 +9419,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="253" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="253" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="7" t="s">
         <v>12</v>
       </c>
@@ -9437,7 +9437,7 @@
         <v>70</v>
       </c>
       <c r="G253" s="11" t="n">
-        <v>86122125</v>
+        <v>153106000</v>
       </c>
       <c r="H253" s="5" t="s">
         <v>23</v>
@@ -9455,7 +9455,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="254" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="254" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="7" t="s">
         <v>12</v>
       </c>
@@ -9473,7 +9473,7 @@
         <v>75</v>
       </c>
       <c r="G254" s="11" t="n">
-        <v>118858500</v>
+        <v>211304000</v>
       </c>
       <c r="H254" s="5" t="s">
         <v>23</v>
@@ -9491,7 +9491,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="255" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="255" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="7" t="s">
         <v>12</v>
       </c>
@@ -9509,7 +9509,7 @@
         <v>80</v>
       </c>
       <c r="G255" s="11" t="n">
-        <v>164003062.5</v>
+        <v>291561000</v>
       </c>
       <c r="H255" s="5" t="s">
         <v>23</v>
@@ -9527,7 +9527,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="256" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="256" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="7" t="s">
         <v>12</v>
       </c>
@@ -9545,7 +9545,7 @@
         <v>85</v>
       </c>
       <c r="G256" s="11" t="n">
-        <v>226308375</v>
+        <v>402326000</v>
       </c>
       <c r="H256" s="5" t="s">
         <v>23</v>
@@ -9563,7 +9563,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="257" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="257" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="7" t="s">
         <v>12</v>
       </c>
@@ -9581,7 +9581,7 @@
         <v>90</v>
       </c>
       <c r="G257" s="11" t="n">
-        <v>312292125</v>
+        <v>555186000</v>
       </c>
       <c r="H257" s="5" t="s">
         <v>23</v>
@@ -9599,7 +9599,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="258" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="258" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="7" t="s">
         <v>20</v>
       </c>
@@ -9617,7 +9617,7 @@
         <v>5</v>
       </c>
       <c r="G258" s="10" t="n">
-        <v>19986750</v>
+        <v>35532000</v>
       </c>
       <c r="H258" s="5" t="s">
         <v>23</v>
@@ -9635,7 +9635,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="259" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="259" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="7" t="s">
         <v>20</v>
       </c>
@@ -9653,7 +9653,7 @@
         <v>18</v>
       </c>
       <c r="G259" s="10" t="n">
-        <v>17376750</v>
+        <v>30892000</v>
       </c>
       <c r="H259" s="5" t="s">
         <v>23</v>
@@ -9671,7 +9671,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="260" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="260" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="7" t="s">
         <v>20</v>
       </c>
@@ -9689,7 +9689,7 @@
         <v>25</v>
       </c>
       <c r="G260" s="10" t="n">
-        <v>28298250</v>
+        <v>50308000</v>
       </c>
       <c r="H260" s="5" t="s">
         <v>23</v>
@@ -9707,7 +9707,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="261" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="261" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="7" t="s">
         <v>20</v>
       </c>
@@ -9725,7 +9725,7 @@
         <v>30</v>
       </c>
       <c r="G261" s="10" t="n">
-        <v>30420000</v>
+        <v>54080000</v>
       </c>
       <c r="H261" s="5" t="s">
         <v>23</v>
@@ -9743,7 +9743,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="262" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="262" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="7" t="s">
         <v>20</v>
       </c>
@@ -9761,7 +9761,7 @@
         <v>35</v>
       </c>
       <c r="G262" s="10" t="n">
-        <v>32542312.5</v>
+        <v>57853000</v>
       </c>
       <c r="H262" s="5" t="s">
         <v>23</v>
@@ -9779,7 +9779,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="263" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="263" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="7" t="s">
         <v>20</v>
       </c>
@@ -9797,7 +9797,7 @@
         <v>40</v>
       </c>
       <c r="G263" s="10" t="n">
-        <v>34788937.5</v>
+        <v>61847000</v>
       </c>
       <c r="H263" s="5" t="s">
         <v>23</v>
@@ -9815,7 +9815,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="264" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="264" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="7" t="s">
         <v>20</v>
       </c>
@@ -9833,7 +9833,7 @@
         <v>45</v>
       </c>
       <c r="G264" s="10" t="n">
-        <v>36536625</v>
+        <v>64954000</v>
       </c>
       <c r="H264" s="5" t="s">
         <v>23</v>
@@ -9851,7 +9851,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="265" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="265" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="7" t="s">
         <v>20</v>
       </c>
@@ -9869,7 +9869,7 @@
         <v>50</v>
       </c>
       <c r="G265" s="10" t="n">
-        <v>41337562.5</v>
+        <v>73489000</v>
       </c>
       <c r="H265" s="5" t="s">
         <v>23</v>
@@ -9887,7 +9887,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="266" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="266" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="7" t="s">
         <v>20</v>
       </c>
@@ -9905,7 +9905,7 @@
         <v>55</v>
       </c>
       <c r="G266" s="10" t="n">
-        <v>46340437.5</v>
+        <v>82383000</v>
       </c>
       <c r="H266" s="5" t="s">
         <v>23</v>
@@ -9923,7 +9923,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="267" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="267" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="7" t="s">
         <v>20</v>
       </c>
@@ -9941,7 +9941,7 @@
         <v>60</v>
       </c>
       <c r="G267" s="11" t="n">
-        <v>57039750</v>
+        <v>101404000</v>
       </c>
       <c r="H267" s="5" t="s">
         <v>23</v>
@@ -9959,7 +9959,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="268" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="268" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="7" t="s">
         <v>20</v>
       </c>
@@ -9977,7 +9977,7 @@
         <v>65</v>
       </c>
       <c r="G268" s="11" t="n">
-        <v>68447812.5</v>
+        <v>121685000</v>
       </c>
       <c r="H268" s="5" t="s">
         <v>23</v>
@@ -9995,7 +9995,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="269" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="269" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="7" t="s">
         <v>20</v>
       </c>
@@ -10013,7 +10013,7 @@
         <v>70</v>
       </c>
       <c r="G269" s="11" t="n">
-        <v>102660187.5</v>
+        <v>182507000</v>
       </c>
       <c r="H269" s="5" t="s">
         <v>23</v>
@@ -10031,7 +10031,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="270" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="270" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="7" t="s">
         <v>20</v>
       </c>
@@ -10049,7 +10049,7 @@
         <v>75</v>
       </c>
       <c r="G270" s="11" t="n">
-        <v>141692625</v>
+        <v>251898000</v>
       </c>
       <c r="H270" s="5" t="s">
         <v>23</v>
@@ -10067,7 +10067,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="271" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="271" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="7" t="s">
         <v>20</v>
       </c>
@@ -10085,7 +10085,7 @@
         <v>80</v>
       </c>
       <c r="G271" s="11" t="n">
-        <v>195547500</v>
+        <v>347640000</v>
       </c>
       <c r="H271" s="5" t="s">
         <v>23</v>
@@ -10103,7 +10103,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="272" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="272" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="7" t="s">
         <v>20</v>
       </c>
@@ -10121,7 +10121,7 @@
         <v>85</v>
       </c>
       <c r="G272" s="11" t="n">
-        <v>269859375</v>
+        <v>479750000</v>
       </c>
       <c r="H272" s="5" t="s">
         <v>23</v>
@@ -10139,7 +10139,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="273" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="273" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="7" t="s">
         <v>20</v>
       </c>
@@ -10157,7 +10157,7 @@
         <v>90</v>
       </c>
       <c r="G273" s="11" t="n">
-        <v>372390750</v>
+        <v>662028000</v>
       </c>
       <c r="H273" s="5" t="s">
         <v>23</v>
@@ -10175,7 +10175,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="274" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="274" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="7" t="s">
         <v>21</v>
       </c>
@@ -10193,7 +10193,7 @@
         <v>5</v>
       </c>
       <c r="G274" s="10" t="n">
-        <v>22884750</v>
+        <v>40684000</v>
       </c>
       <c r="H274" s="5" t="s">
         <v>23</v>
@@ -10211,7 +10211,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="275" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="275" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="7" t="s">
         <v>21</v>
       </c>
@@ -10229,7 +10229,7 @@
         <v>18</v>
       </c>
       <c r="G275" s="10" t="n">
-        <v>19895625</v>
+        <v>35370000</v>
       </c>
       <c r="H275" s="5" t="s">
         <v>23</v>
@@ -10247,7 +10247,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="276" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="276" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="7" t="s">
         <v>21</v>
       </c>
@@ -10265,7 +10265,7 @@
         <v>25</v>
       </c>
       <c r="G276" s="10" t="n">
-        <v>35816062.5</v>
+        <v>63673000</v>
       </c>
       <c r="H276" s="5" t="s">
         <v>23</v>
@@ -10283,7 +10283,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="277" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="277" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="7" t="s">
         <v>21</v>
       </c>
@@ -10301,7 +10301,7 @@
         <v>30</v>
       </c>
       <c r="G277" s="10" t="n">
-        <v>38370375</v>
+        <v>68214000</v>
       </c>
       <c r="H277" s="5" t="s">
         <v>23</v>
@@ -10319,7 +10319,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="278" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="278" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="7" t="s">
         <v>21</v>
       </c>
@@ -10337,7 +10337,7 @@
         <v>35</v>
       </c>
       <c r="G278" s="10" t="n">
-        <v>40960125</v>
+        <v>72818000</v>
       </c>
       <c r="H278" s="5" t="s">
         <v>23</v>
@@ -10355,7 +10355,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="279" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="279" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="7" t="s">
         <v>21</v>
       </c>
@@ -10373,7 +10373,7 @@
         <v>40</v>
       </c>
       <c r="G279" s="10" t="n">
-        <v>43521750</v>
+        <v>77372000</v>
       </c>
       <c r="H279" s="5" t="s">
         <v>23</v>
@@ -10391,7 +10391,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="280" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="280" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="7" t="s">
         <v>21</v>
       </c>
@@ -10409,7 +10409,7 @@
         <v>45</v>
       </c>
       <c r="G280" s="10" t="n">
-        <v>46932750</v>
+        <v>83436000</v>
       </c>
       <c r="H280" s="5" t="s">
         <v>23</v>
@@ -10427,7 +10427,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="281" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="281" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="7" t="s">
         <v>21</v>
       </c>
@@ -10445,7 +10445,7 @@
         <v>50</v>
       </c>
       <c r="G281" s="10" t="n">
-        <v>49560187.5</v>
+        <v>88107000</v>
       </c>
       <c r="H281" s="5" t="s">
         <v>23</v>
@@ -10463,7 +10463,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="282" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="282" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="7" t="s">
         <v>21</v>
       </c>
@@ -10481,7 +10481,7 @@
         <v>55</v>
       </c>
       <c r="G282" s="11" t="n">
-        <v>57004875</v>
+        <v>101342000</v>
       </c>
       <c r="H282" s="5" t="s">
         <v>23</v>
@@ -10499,7 +10499,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="283" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="283" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="7" t="s">
         <v>21</v>
       </c>
@@ -10517,7 +10517,7 @@
         <v>60</v>
       </c>
       <c r="G283" s="11" t="n">
-        <v>64145812.5</v>
+        <v>114037000</v>
       </c>
       <c r="H283" s="5" t="s">
         <v>23</v>
@@ -10535,7 +10535,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="284" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="284" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="7" t="s">
         <v>21</v>
       </c>
@@ -10553,7 +10553,7 @@
         <v>65</v>
       </c>
       <c r="G284" s="11" t="n">
-        <v>88701750</v>
+        <v>157692000</v>
       </c>
       <c r="H284" s="5" t="s">
         <v>23</v>
@@ -10571,7 +10571,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="285" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="285" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="7" t="s">
         <v>21</v>
       </c>
@@ -10589,7 +10589,7 @@
         <v>70</v>
       </c>
       <c r="G285" s="11" t="n">
-        <v>119752875</v>
+        <v>212894000</v>
       </c>
       <c r="H285" s="5" t="s">
         <v>23</v>
@@ -10607,7 +10607,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="286" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="286" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="7" t="s">
         <v>21</v>
       </c>
@@ -10625,7 +10625,7 @@
         <v>75</v>
       </c>
       <c r="G286" s="11" t="n">
-        <v>168168937.5</v>
+        <v>298967000</v>
       </c>
       <c r="H286" s="5" t="s">
         <v>23</v>
@@ -10643,7 +10643,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="287" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="287" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="7" t="s">
         <v>21</v>
       </c>
@@ -10661,7 +10661,7 @@
         <v>80</v>
       </c>
       <c r="G287" s="11" t="n">
-        <v>233926312.5</v>
+        <v>415869000</v>
       </c>
       <c r="H287" s="5" t="s">
         <v>23</v>
@@ -10679,7 +10679,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="288" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="288" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="7" t="s">
         <v>21</v>
       </c>
@@ -10697,7 +10697,7 @@
         <v>85</v>
       </c>
       <c r="G288" s="11" t="n">
-        <v>327496500</v>
+        <v>582216000</v>
       </c>
       <c r="H288" s="5" t="s">
         <v>23</v>
@@ -10715,7 +10715,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="289" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="289" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="7" t="s">
         <v>21</v>
       </c>
@@ -10733,7 +10733,7 @@
         <v>90</v>
       </c>
       <c r="G289" s="11" t="n">
-        <v>458494875</v>
+        <v>815102000</v>
       </c>
       <c r="H289" s="5" t="s">
         <v>23</v>

</xml_diff>